<commit_message>
Meeting mins 16/12/18 + updated christmas availability spreadsheet
</commit_message>
<xml_diff>
--- a/Admin/Group Chistmas Avaliability.xlsx
+++ b/Admin/Group Chistmas Avaliability.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomgi\Documents\GitHub\game-project-group-3\Admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\_GitHub\game-project-group-3\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AD801D75-812F-4D62-94C8-E5B39F5C3EB9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{00B8C396-0C9C-437A-A0FB-3ECB1F5D1F70}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -435,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -451,9 +451,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -486,6 +484,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -803,7 +802,7 @@
   <dimension ref="A1:S54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,65 +821,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="M1" s="36"/>
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="33" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="36"/>
+      <c r="M2" s="34"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
+      <c r="A3" s="25"/>
       <c r="B3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="19"/>
-      <c r="K3" s="34" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="17"/>
+      <c r="K3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="36"/>
+      <c r="M3" s="34"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="10" t="s">
         <v>18</v>
       </c>
@@ -890,31 +889,31 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
-      <c r="I4" s="20"/>
+      <c r="I4" s="18"/>
       <c r="K4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="36"/>
+      <c r="M4" s="34"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="20"/>
+      <c r="I5" s="21"/>
       <c r="K5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="36"/>
+      <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="27"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="10" t="s">
         <v>21</v>
       </c>
@@ -924,14 +923,14 @@
       <c r="F6" s="4"/>
       <c r="G6" s="3"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="23"/>
+      <c r="I6" s="21"/>
       <c r="K6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="36"/>
+      <c r="M6" s="34"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="10" t="s">
         <v>22</v>
       </c>
@@ -941,11 +940,11 @@
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="20"/>
-      <c r="M7" s="36"/>
+      <c r="I7" s="18"/>
+      <c r="M7" s="34"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="10" t="s">
         <v>23</v>
       </c>
@@ -955,14 +954,14 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="20"/>
-      <c r="K8" s="35" t="s">
+      <c r="I8" s="18"/>
+      <c r="K8" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="M8" s="36"/>
+      <c r="M8" s="34"/>
     </row>
     <row r="9" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="27"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="11" t="s">
         <v>24</v>
       </c>
@@ -972,117 +971,117 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-      <c r="I9" s="22"/>
+      <c r="I9" s="20"/>
       <c r="K9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M9" s="36"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="30"/>
+      <c r="M9" s="34"/>
+      <c r="Q9" s="28"/>
+      <c r="R9" s="28"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="M10" s="36"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="29"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="M10" s="34"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="27"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36"/>
-      <c r="M11" s="36"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="30"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
     </row>
     <row r="12" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="28"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
-      <c r="M12" s="36"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="30"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="25"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="M12" s="34"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
     </row>
     <row r="13" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27"/>
-      <c r="B13" s="33" t="s">
+      <c r="A13" s="25"/>
+      <c r="B13" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="17" t="s">
+      <c r="E13" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="17" t="s">
+      <c r="F13" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I13" s="18" t="s">
+      <c r="I13" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="J13" s="27"/>
-      <c r="K13" s="34" t="s">
+      <c r="J13" s="25"/>
+      <c r="K13" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="M13" s="36"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="30"/>
+      <c r="M13" s="34"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="27"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="25"/>
       <c r="K14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M14" s="36"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
+      <c r="M14" s="34"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="10" t="s">
         <v>18</v>
       </c>
@@ -1092,17 +1091,17 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="26" t="s">
+      <c r="I15" s="18"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="M15" s="36"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="30"/>
+      <c r="M15" s="34"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="27"/>
+      <c r="A16" s="25"/>
       <c r="B16" s="10" t="s">
         <v>20</v>
       </c>
@@ -1110,19 +1109,19 @@
       <c r="D16" s="4"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="32" t="s">
+      <c r="I16" s="21"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="36"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="30"/>
+      <c r="M16" s="34"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="10" t="s">
         <v>21</v>
       </c>
@@ -1132,34 +1131,34 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="27"/>
-      <c r="M17" s="36"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="30"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="25"/>
+      <c r="M17" s="34"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="37"/>
+      <c r="E18" s="35"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="35" t="s">
+      <c r="I18" s="18"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="M18" s="36"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="30"/>
+      <c r="M18" s="34"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="10" t="s">
         <v>23</v>
       </c>
@@ -1169,128 +1168,128 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="27"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="25"/>
       <c r="K19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M19" s="36"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="30"/>
+      <c r="M19" s="34"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="28"/>
     </row>
     <row r="20" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="24"/>
+      <c r="C20" s="22"/>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="6"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="27"/>
-      <c r="M20" s="36"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="30"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="25"/>
+      <c r="M20" s="34"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="28"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A21" s="27"/>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="M21" s="36"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
+      <c r="A21" s="25"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="M21" s="34"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="31"/>
-      <c r="B22" s="31"/>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="31"/>
-      <c r="I22" s="31"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
-      <c r="M22" s="36"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="30"/>
+      <c r="A22" s="29"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="M23" s="25"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="29"/>
+      <c r="A23" s="25"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="M23" s="23"/>
+      <c r="Q23" s="28"/>
+      <c r="R23" s="27"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
-      <c r="B24" s="27"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="Q24" s="30"/>
-      <c r="R24" s="30"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="Q25" s="30"/>
-      <c r="R25" s="30"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="28"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="27"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="25"/>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="25"/>
+      <c r="F26" s="25"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B28" s="1"/>
@@ -1300,393 +1299,393 @@
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
-      <c r="Q28" s="30"/>
-      <c r="R28" s="30"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="28"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q29" s="30"/>
-      <c r="R29" s="30"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q30" s="30"/>
-      <c r="R30" s="30"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="28"/>
     </row>
     <row r="33" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
-      <c r="J33" s="27"/>
-      <c r="K33" s="27"/>
-      <c r="L33" s="27"/>
-      <c r="M33" s="27"/>
-      <c r="N33" s="27"/>
-      <c r="O33" s="27"/>
-      <c r="P33" s="27"/>
-      <c r="Q33" s="27"/>
-      <c r="R33" s="27"/>
-      <c r="S33" s="27"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+      <c r="O33" s="25"/>
+      <c r="P33" s="25"/>
+      <c r="Q33" s="25"/>
+      <c r="R33" s="25"/>
+      <c r="S33" s="25"/>
     </row>
     <row r="34" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
-      <c r="G34" s="27"/>
-      <c r="H34" s="27"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="27"/>
-      <c r="M34" s="27"/>
-      <c r="N34" s="27"/>
-      <c r="O34" s="27"/>
-      <c r="P34" s="27"/>
-      <c r="Q34" s="27"/>
-      <c r="R34" s="27"/>
-      <c r="S34" s="27"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+      <c r="O34" s="25"/>
+      <c r="P34" s="25"/>
+      <c r="Q34" s="25"/>
+      <c r="R34" s="25"/>
+      <c r="S34" s="25"/>
     </row>
     <row r="35" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E35" s="27"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="29"/>
-      <c r="H35" s="29"/>
-      <c r="I35" s="29"/>
-      <c r="J35" s="29"/>
-      <c r="K35" s="29"/>
-      <c r="L35" s="29"/>
-      <c r="M35" s="29"/>
-      <c r="N35" s="27"/>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
-      <c r="R35" s="27"/>
-      <c r="S35" s="27"/>
+      <c r="E35" s="25"/>
+      <c r="F35" s="26"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
+      <c r="L35" s="27"/>
+      <c r="M35" s="27"/>
+      <c r="N35" s="25"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="25"/>
+      <c r="S35" s="25"/>
     </row>
     <row r="36" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E36" s="27"/>
-      <c r="F36" s="27"/>
-      <c r="G36" s="27"/>
-      <c r="H36" s="27"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="27"/>
-      <c r="M36" s="27"/>
-      <c r="N36" s="27"/>
-      <c r="O36" s="29"/>
-      <c r="P36" s="27"/>
-      <c r="Q36" s="27"/>
-      <c r="R36" s="27"/>
-      <c r="S36" s="27"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+      <c r="O36" s="27"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="25"/>
+      <c r="R36" s="25"/>
+      <c r="S36" s="25"/>
     </row>
     <row r="37" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E37" s="27"/>
-      <c r="F37" s="27"/>
-      <c r="G37" s="27"/>
-      <c r="H37" s="27"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-      <c r="O37" s="27"/>
-      <c r="P37" s="27"/>
-      <c r="Q37" s="27"/>
-      <c r="R37" s="27"/>
-      <c r="S37" s="27"/>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="25"/>
+      <c r="O37" s="25"/>
+      <c r="P37" s="25"/>
+      <c r="Q37" s="25"/>
+      <c r="R37" s="25"/>
+      <c r="S37" s="25"/>
     </row>
     <row r="38" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="27"/>
-      <c r="R38" s="27"/>
-      <c r="S38" s="27"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="25"/>
+      <c r="O38" s="25"/>
+      <c r="P38" s="25"/>
+      <c r="Q38" s="25"/>
+      <c r="R38" s="25"/>
+      <c r="S38" s="25"/>
     </row>
     <row r="39" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
-      <c r="Q39" s="27"/>
-      <c r="R39" s="27"/>
-      <c r="S39" s="27"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+      <c r="O39" s="25"/>
+      <c r="P39" s="25"/>
+      <c r="Q39" s="25"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
     </row>
     <row r="40" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
-      <c r="M40" s="27"/>
-      <c r="N40" s="27"/>
-      <c r="O40" s="27"/>
-      <c r="P40" s="27"/>
-      <c r="Q40" s="27"/>
-      <c r="R40" s="27"/>
-      <c r="S40" s="27"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+      <c r="O40" s="25"/>
+      <c r="P40" s="25"/>
+      <c r="Q40" s="25"/>
+      <c r="R40" s="25"/>
+      <c r="S40" s="25"/>
     </row>
     <row r="41" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
-      <c r="Q41" s="27"/>
-      <c r="R41" s="27"/>
-      <c r="S41" s="27"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+      <c r="O41" s="25"/>
+      <c r="P41" s="25"/>
+      <c r="Q41" s="25"/>
+      <c r="R41" s="25"/>
+      <c r="S41" s="25"/>
     </row>
     <row r="42" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="29"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
-      <c r="M42" s="27"/>
-      <c r="N42" s="27"/>
-      <c r="O42" s="27"/>
-      <c r="P42" s="27"/>
-      <c r="Q42" s="27"/>
-      <c r="R42" s="27"/>
-      <c r="S42" s="27"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="25"/>
+      <c r="P42" s="25"/>
+      <c r="Q42" s="25"/>
+      <c r="R42" s="25"/>
+      <c r="S42" s="25"/>
     </row>
     <row r="43" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
-      <c r="M43" s="27"/>
-      <c r="N43" s="27"/>
-      <c r="O43" s="27"/>
-      <c r="P43" s="27"/>
-      <c r="Q43" s="27"/>
-      <c r="R43" s="27"/>
-      <c r="S43" s="27"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+      <c r="O43" s="25"/>
+      <c r="P43" s="25"/>
+      <c r="Q43" s="25"/>
+      <c r="R43" s="25"/>
+      <c r="S43" s="25"/>
     </row>
     <row r="44" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
-      <c r="M44" s="27"/>
-      <c r="N44" s="27"/>
-      <c r="O44" s="27"/>
-      <c r="P44" s="27"/>
-      <c r="Q44" s="27"/>
-      <c r="R44" s="27"/>
-      <c r="S44" s="27"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+      <c r="O44" s="25"/>
+      <c r="P44" s="25"/>
+      <c r="Q44" s="25"/>
+      <c r="R44" s="25"/>
+      <c r="S44" s="25"/>
     </row>
     <row r="45" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="27"/>
-      <c r="L45" s="27"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="27"/>
-      <c r="P45" s="27"/>
-      <c r="Q45" s="27"/>
-      <c r="R45" s="27"/>
-      <c r="S45" s="27"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="25"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="25"/>
+      <c r="O45" s="25"/>
+      <c r="P45" s="25"/>
+      <c r="Q45" s="25"/>
+      <c r="R45" s="25"/>
+      <c r="S45" s="25"/>
     </row>
     <row r="46" spans="2:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="E46" s="27"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="29"/>
-      <c r="K46" s="29"/>
-      <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
-      <c r="N46" s="27"/>
-      <c r="O46" s="29"/>
-      <c r="P46" s="27"/>
-      <c r="Q46" s="27"/>
-      <c r="R46" s="27"/>
-      <c r="S46" s="27"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+      <c r="N46" s="25"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="25"/>
+      <c r="Q46" s="25"/>
+      <c r="R46" s="25"/>
+      <c r="S46" s="25"/>
     </row>
     <row r="47" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
-      <c r="M47" s="27"/>
-      <c r="N47" s="27"/>
-      <c r="O47" s="27"/>
-      <c r="P47" s="27"/>
-      <c r="Q47" s="27"/>
-      <c r="R47" s="27"/>
-      <c r="S47" s="27"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="25"/>
+      <c r="K47" s="25"/>
+      <c r="L47" s="25"/>
+      <c r="M47" s="25"/>
+      <c r="N47" s="25"/>
+      <c r="O47" s="25"/>
+      <c r="P47" s="25"/>
+      <c r="Q47" s="25"/>
+      <c r="R47" s="25"/>
+      <c r="S47" s="25"/>
     </row>
     <row r="48" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
-      <c r="O48" s="27"/>
-      <c r="P48" s="27"/>
-      <c r="Q48" s="27"/>
-      <c r="R48" s="27"/>
-      <c r="S48" s="27"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="25"/>
+      <c r="N48" s="25"/>
+      <c r="O48" s="25"/>
+      <c r="P48" s="25"/>
+      <c r="Q48" s="25"/>
+      <c r="R48" s="25"/>
+      <c r="S48" s="25"/>
     </row>
     <row r="49" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="27"/>
-      <c r="M49" s="27"/>
-      <c r="N49" s="27"/>
-      <c r="O49" s="27"/>
-      <c r="P49" s="27"/>
-      <c r="Q49" s="27"/>
-      <c r="R49" s="27"/>
-      <c r="S49" s="27"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="25"/>
+      <c r="O49" s="25"/>
+      <c r="P49" s="25"/>
+      <c r="Q49" s="25"/>
+      <c r="R49" s="25"/>
+      <c r="S49" s="25"/>
     </row>
     <row r="50" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
-      <c r="L50" s="27"/>
-      <c r="M50" s="27"/>
-      <c r="N50" s="27"/>
-      <c r="O50" s="27"/>
-      <c r="P50" s="27"/>
-      <c r="Q50" s="27"/>
-      <c r="R50" s="27"/>
-      <c r="S50" s="27"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="25"/>
+      <c r="O50" s="25"/>
+      <c r="P50" s="25"/>
+      <c r="Q50" s="25"/>
+      <c r="R50" s="25"/>
+      <c r="S50" s="25"/>
     </row>
     <row r="51" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="27"/>
-      <c r="L51" s="27"/>
-      <c r="M51" s="27"/>
-      <c r="N51" s="27"/>
-      <c r="O51" s="27"/>
-      <c r="P51" s="27"/>
-      <c r="Q51" s="27"/>
-      <c r="R51" s="27"/>
-      <c r="S51" s="27"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="25"/>
+      <c r="O51" s="25"/>
+      <c r="P51" s="25"/>
+      <c r="Q51" s="25"/>
+      <c r="R51" s="25"/>
+      <c r="S51" s="25"/>
     </row>
     <row r="52" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
-      <c r="G52" s="27"/>
-      <c r="H52" s="27"/>
-      <c r="I52" s="27"/>
-      <c r="J52" s="27"/>
-      <c r="K52" s="27"/>
-      <c r="L52" s="27"/>
-      <c r="M52" s="27"/>
-      <c r="N52" s="27"/>
-      <c r="O52" s="27"/>
-      <c r="P52" s="27"/>
-      <c r="Q52" s="27"/>
-      <c r="R52" s="27"/>
-      <c r="S52" s="27"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="25"/>
+      <c r="O52" s="25"/>
+      <c r="P52" s="25"/>
+      <c r="Q52" s="25"/>
+      <c r="R52" s="25"/>
+      <c r="S52" s="25"/>
     </row>
     <row r="53" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E53" s="27"/>
-      <c r="F53" s="27"/>
-      <c r="G53" s="27"/>
-      <c r="H53" s="27"/>
-      <c r="I53" s="27"/>
-      <c r="J53" s="27"/>
-      <c r="K53" s="27"/>
-      <c r="L53" s="27"/>
-      <c r="M53" s="27"/>
-      <c r="N53" s="27"/>
-      <c r="O53" s="27"/>
-      <c r="P53" s="27"/>
-      <c r="Q53" s="27"/>
-      <c r="R53" s="27"/>
-      <c r="S53" s="27"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+      <c r="O53" s="25"/>
+      <c r="P53" s="25"/>
+      <c r="Q53" s="25"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="25"/>
     </row>
     <row r="54" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="27"/>
-      <c r="K54" s="27"/>
-      <c r="L54" s="27"/>
-      <c r="M54" s="27"/>
-      <c r="N54" s="27"/>
-      <c r="O54" s="27"/>
-      <c r="P54" s="27"/>
-      <c r="Q54" s="27"/>
-      <c r="R54" s="27"/>
-      <c r="S54" s="27"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="25"/>
+      <c r="O54" s="25"/>
+      <c r="P54" s="25"/>
+      <c r="Q54" s="25"/>
+      <c r="R54" s="25"/>
+      <c r="S54" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Team Christmas availability updated as per meeting 8.1.19
</commit_message>
<xml_diff>
--- a/Admin/Group Chistmas Avaliability.xlsx
+++ b/Admin/Group Chistmas Avaliability.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\_GitHub\game-project-group-3\Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{00B8C396-0C9C-437A-A0FB-3ECB1F5D1F70}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{64D381E2-3862-42C4-A9A6-A7F70338154C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -801,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,12 +935,12 @@
         <v>22</v>
       </c>
       <c r="C7" s="7"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="3"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="18"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="21"/>
       <c r="M7" s="34"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -1128,8 +1128,8 @@
       <c r="C17" s="7"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="18"/>
       <c r="J17" s="25"/>
@@ -1143,7 +1143,7 @@
         <v>22</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="D18" s="3"/>
+      <c r="D18" s="4"/>
       <c r="E18" s="35"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1166,7 +1166,7 @@
       <c r="D19" s="4"/>
       <c r="E19" s="3"/>
       <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="G19" s="3"/>
       <c r="H19" s="4"/>
       <c r="I19" s="18"/>
       <c r="J19" s="25"/>

</xml_diff>